<commit_message>
CLI-Tool for Validation Summary (File based)
</commit_message>
<xml_diff>
--- a/tests/test_data/notice_validator/test_repository/test_package_F03/transformation/conceptual_mappings.xlsx
+++ b/tests/test_data/notice_validator/test_repository/test_package_F03/transformation/conceptual_mappings.xlsx
@@ -195,7 +195,7 @@
     <t xml:space="preserve">ePO mapping</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard Form Field ID (M) </t>
+    <t xml:space="preserve">Standard Form Field ID (M)</t>
   </si>
   <si>
     <t xml:space="preserve">Standard Form Field Name (M)</t>
@@ -6301,7 +6301,7 @@
       <selection pane="bottomLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.63"/>
@@ -9399,7 +9399,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -9444,7 +9444,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -9489,7 +9489,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -9534,7 +9534,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -9579,7 +9579,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -9624,7 +9624,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -9668,10 +9668,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.26"/>
@@ -18876,7 +18876,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.75"/>
@@ -19011,7 +19011,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.38"/>
   </cols>
@@ -19090,7 +19090,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.25"/>
   </cols>
@@ -19163,7 +19163,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45"/>
@@ -19190,7 +19190,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.12"/>
@@ -19296,7 +19296,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>
@@ -19357,7 +19357,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.38"/>

</xml_diff>